<commit_message>
setting the main time test to only run data sets 2 and 3
</commit_message>
<xml_diff>
--- a/Data/timings_both_models_16-16_treatments.xlsx
+++ b/Data/timings_both_models_16-16_treatments.xlsx
@@ -464,25 +464,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>12.709</v>
+        <v>12.141</v>
       </c>
       <c r="G2">
-        <v>0.356</v>
+        <v>0.342</v>
       </c>
       <c r="H2">
-        <v>8.946</v>
+        <v>8.234999999999999</v>
       </c>
       <c r="I2">
-        <v>1.63</v>
+        <v>1.717</v>
       </c>
       <c r="J2">
-        <v>1.627</v>
+        <v>1.722</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00085</v>
+        <v>0.0009300000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -502,25 +502,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>12.739</v>
+        <v>13.079</v>
       </c>
       <c r="G3">
         <v>0.348</v>
       </c>
       <c r="H3">
-        <v>8.926</v>
+        <v>9.087999999999999</v>
       </c>
       <c r="I3">
-        <v>1.669</v>
+        <v>1.729</v>
       </c>
       <c r="J3">
-        <v>1.667</v>
+        <v>1.767</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00085</v>
+        <v>0.00088</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -540,25 +540,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>12.677</v>
+        <v>13.631</v>
       </c>
       <c r="G4">
-        <v>0.355</v>
+        <v>0.376</v>
       </c>
       <c r="H4">
-        <v>8.888999999999999</v>
+        <v>9.420999999999999</v>
       </c>
       <c r="I4">
-        <v>1.676</v>
+        <v>1.833</v>
       </c>
       <c r="J4">
-        <v>1.628</v>
+        <v>1.853</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00085</v>
+        <v>0.00108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -578,25 +578,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>12.787</v>
+        <v>16.754</v>
       </c>
       <c r="G5">
-        <v>0.357</v>
+        <v>0.448</v>
       </c>
       <c r="H5">
-        <v>9.010999999999999</v>
+        <v>12.085</v>
       </c>
       <c r="I5">
-        <v>1.659</v>
+        <v>2.076</v>
       </c>
       <c r="J5">
-        <v>1.632</v>
+        <v>1.981</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00084</v>
+        <v>0.00102</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -616,25 +616,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>12.69</v>
+        <v>15.019</v>
       </c>
       <c r="G6">
-        <v>0.349</v>
+        <v>0.483</v>
       </c>
       <c r="H6">
-        <v>8.923999999999999</v>
+        <v>10.445</v>
       </c>
       <c r="I6">
-        <v>1.664</v>
+        <v>2.046</v>
       </c>
       <c r="J6">
-        <v>1.625</v>
+        <v>1.905</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00085</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -702,25 +702,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>12.67</v>
+        <v>13.2</v>
       </c>
       <c r="G2">
-        <v>0.007</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="H2">
-        <v>0.011</v>
+        <v>0.02</v>
       </c>
       <c r="I2">
-        <v>5.561</v>
+        <v>5.597</v>
       </c>
       <c r="J2">
-        <v>5.576</v>
+        <v>5.732</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00086</v>
+        <v>0.00117</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -740,25 +740,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>12.796</v>
+        <v>13.951</v>
       </c>
       <c r="G3">
-        <v>0.007</v>
+        <v>0.011</v>
       </c>
       <c r="H3">
-        <v>0.012</v>
+        <v>0.02</v>
       </c>
       <c r="I3">
-        <v>5.588</v>
+        <v>5.974</v>
       </c>
       <c r="J3">
-        <v>5.632</v>
+        <v>5.815</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00086</v>
+        <v>0.00106</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -778,25 +778,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>12.961</v>
+        <v>13.277</v>
       </c>
       <c r="G4">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="H4">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="I4">
-        <v>5.568</v>
+        <v>5.692</v>
       </c>
       <c r="J4">
-        <v>5.872</v>
+        <v>5.658</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00088</v>
+        <v>0.00103</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -816,25 +816,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>12.725</v>
+        <v>13.067</v>
       </c>
       <c r="G5">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="H5">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="I5">
-        <v>5.567</v>
+        <v>5.523</v>
       </c>
       <c r="J5">
-        <v>5.593</v>
+        <v>5.716</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00086</v>
+        <v>0.0011</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -854,25 +854,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>12.663</v>
+        <v>13.976</v>
       </c>
       <c r="G6">
-        <v>0.007</v>
+        <v>0.01</v>
       </c>
       <c r="H6">
-        <v>0.012</v>
+        <v>0.02</v>
       </c>
       <c r="I6">
-        <v>5.567</v>
+        <v>6.134</v>
       </c>
       <c r="J6">
-        <v>5.57</v>
+        <v>5.898</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00087</v>
+        <v>0.00108</v>
       </c>
     </row>
   </sheetData>
@@ -940,25 +940,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>12.709</v>
+        <v>12.141</v>
       </c>
       <c r="G2">
-        <v>0.356</v>
+        <v>0.342</v>
       </c>
       <c r="H2">
-        <v>8.946</v>
+        <v>8.234999999999999</v>
       </c>
       <c r="I2">
-        <v>1.63</v>
+        <v>1.717</v>
       </c>
       <c r="J2">
-        <v>1.627</v>
+        <v>1.722</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00085</v>
+        <v>0.0009300000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -978,25 +978,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>12.739</v>
+        <v>13.079</v>
       </c>
       <c r="G3">
         <v>0.348</v>
       </c>
       <c r="H3">
-        <v>8.926</v>
+        <v>9.087999999999999</v>
       </c>
       <c r="I3">
-        <v>1.669</v>
+        <v>1.729</v>
       </c>
       <c r="J3">
-        <v>1.667</v>
+        <v>1.767</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00085</v>
+        <v>0.00088</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1016,25 +1016,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>12.677</v>
+        <v>13.631</v>
       </c>
       <c r="G4">
-        <v>0.355</v>
+        <v>0.376</v>
       </c>
       <c r="H4">
-        <v>8.888999999999999</v>
+        <v>9.420999999999999</v>
       </c>
       <c r="I4">
-        <v>1.676</v>
+        <v>1.833</v>
       </c>
       <c r="J4">
-        <v>1.628</v>
+        <v>1.853</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00085</v>
+        <v>0.00108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1054,25 +1054,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>12.787</v>
+        <v>16.754</v>
       </c>
       <c r="G5">
-        <v>0.357</v>
+        <v>0.448</v>
       </c>
       <c r="H5">
-        <v>9.010999999999999</v>
+        <v>12.085</v>
       </c>
       <c r="I5">
-        <v>1.659</v>
+        <v>2.076</v>
       </c>
       <c r="J5">
-        <v>1.632</v>
+        <v>1.981</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00084</v>
+        <v>0.00102</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1092,25 +1092,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>12.69</v>
+        <v>15.019</v>
       </c>
       <c r="G6">
-        <v>0.349</v>
+        <v>0.483</v>
       </c>
       <c r="H6">
-        <v>8.923999999999999</v>
+        <v>10.445</v>
       </c>
       <c r="I6">
-        <v>1.664</v>
+        <v>2.046</v>
       </c>
       <c r="J6">
-        <v>1.625</v>
+        <v>1.905</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00085</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1130,25 +1130,25 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>12.67</v>
+        <v>13.2</v>
       </c>
       <c r="G7">
-        <v>0.007</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="H7">
-        <v>0.011</v>
+        <v>0.02</v>
       </c>
       <c r="I7">
-        <v>5.561</v>
+        <v>5.597</v>
       </c>
       <c r="J7">
-        <v>5.576</v>
+        <v>5.732</v>
       </c>
       <c r="K7">
         <v>1000</v>
       </c>
       <c r="L7">
-        <v>0.00086</v>
+        <v>0.00117</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1168,25 +1168,25 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>12.796</v>
+        <v>13.951</v>
       </c>
       <c r="G8">
-        <v>0.007</v>
+        <v>0.011</v>
       </c>
       <c r="H8">
-        <v>0.012</v>
+        <v>0.02</v>
       </c>
       <c r="I8">
-        <v>5.588</v>
+        <v>5.974</v>
       </c>
       <c r="J8">
-        <v>5.632</v>
+        <v>5.815</v>
       </c>
       <c r="K8">
         <v>1000</v>
       </c>
       <c r="L8">
-        <v>0.00086</v>
+        <v>0.00106</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1206,25 +1206,25 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>12.961</v>
+        <v>13.277</v>
       </c>
       <c r="G9">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="H9">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="I9">
-        <v>5.568</v>
+        <v>5.692</v>
       </c>
       <c r="J9">
-        <v>5.872</v>
+        <v>5.658</v>
       </c>
       <c r="K9">
         <v>1000</v>
       </c>
       <c r="L9">
-        <v>0.00088</v>
+        <v>0.00103</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1244,25 +1244,25 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>12.725</v>
+        <v>13.067</v>
       </c>
       <c r="G10">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="H10">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="I10">
-        <v>5.567</v>
+        <v>5.523</v>
       </c>
       <c r="J10">
-        <v>5.593</v>
+        <v>5.716</v>
       </c>
       <c r="K10">
         <v>1000</v>
       </c>
       <c r="L10">
-        <v>0.00086</v>
+        <v>0.0011</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1282,25 +1282,25 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>12.663</v>
+        <v>13.976</v>
       </c>
       <c r="G11">
-        <v>0.007</v>
+        <v>0.01</v>
       </c>
       <c r="H11">
-        <v>0.012</v>
+        <v>0.02</v>
       </c>
       <c r="I11">
-        <v>5.567</v>
+        <v>6.134</v>
       </c>
       <c r="J11">
-        <v>5.57</v>
+        <v>5.898</v>
       </c>
       <c r="K11">
         <v>1000</v>
       </c>
       <c r="L11">
-        <v>0.00087</v>
+        <v>0.00108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to profile memory and stuff
</commit_message>
<xml_diff>
--- a/Data/timings_both_models_16-16_treatments.xlsx
+++ b/Data/timings_both_models_16-16_treatments.xlsx
@@ -8,15 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Data Set 0 Timings (Pd)" sheetId="1" r:id="rId1"/>
-    <sheet name="Data Set 0 Timings (TD)" sheetId="2" r:id="rId2"/>
-    <sheet name="Data Set 0 Timings (combined)" sheetId="3" r:id="rId3"/>
+    <sheet name="regression - DS 1, T_n 16 (Pd)" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Set 0 Timings (TD)" sheetId="3" r:id="rId3"/>
+    <sheet name="regression - DS 1, T_n 16 (TD)" sheetId="4" r:id="rId4"/>
+    <sheet name="Data Set 0 Timings (combined)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>model</t>
   </si>
@@ -49,6 +51,81 @@
   </si>
   <si>
     <t>Solve Time</t>
+  </si>
+  <si>
+    <t>raw data MRL</t>
+  </si>
+  <si>
+    <t>subset MRL</t>
+  </si>
+  <si>
+    <t>IMPLANT</t>
+  </si>
+  <si>
+    <t>B_MOP</t>
+  </si>
+  <si>
+    <t>B_COP</t>
+  </si>
+  <si>
+    <t>B_COC</t>
+  </si>
+  <si>
+    <t>B_DM</t>
+  </si>
+  <si>
+    <t>POLY_UHWMPE</t>
+  </si>
+  <si>
+    <t>POLY_XPLE</t>
+  </si>
+  <si>
+    <t>POLY_A_XPLE</t>
+  </si>
+  <si>
+    <t>HEAD_22mm</t>
+  </si>
+  <si>
+    <t>HEAD_28mm</t>
+  </si>
+  <si>
+    <t>HEAD_32mm</t>
+  </si>
+  <si>
+    <t>HEAD_36mm</t>
+  </si>
+  <si>
+    <t>HEAD_40mm</t>
+  </si>
+  <si>
+    <t>HEAD_44mm</t>
+  </si>
+  <si>
+    <t>APP_anterior</t>
+  </si>
+  <si>
+    <t>APP_anterolateral</t>
+  </si>
+  <si>
+    <t>APP_posterior</t>
+  </si>
+  <si>
+    <t>APP_transtrochanteric</t>
+  </si>
+  <si>
+    <t>S_VOLLUME</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>R^2 Score</t>
   </si>
 </sst>
 </file>
@@ -464,25 +541,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>12.141</v>
+        <v>11.468</v>
       </c>
       <c r="G2">
-        <v>0.342</v>
+        <v>0.314</v>
       </c>
       <c r="H2">
-        <v>8.234999999999999</v>
+        <v>7.771</v>
       </c>
       <c r="I2">
-        <v>1.717</v>
+        <v>1.65</v>
       </c>
       <c r="J2">
-        <v>1.722</v>
+        <v>1.653</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.0009300000000000001</v>
+        <v>0.00082</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -502,25 +579,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>13.079</v>
+        <v>12.251</v>
       </c>
       <c r="G3">
-        <v>0.348</v>
+        <v>0.329</v>
       </c>
       <c r="H3">
-        <v>9.087999999999999</v>
+        <v>8.461</v>
       </c>
       <c r="I3">
-        <v>1.729</v>
+        <v>1.652</v>
       </c>
       <c r="J3">
-        <v>1.767</v>
+        <v>1.685</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00088</v>
+        <v>0.00086</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -540,25 +617,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>13.631</v>
+        <v>12.68</v>
       </c>
       <c r="G4">
-        <v>0.376</v>
+        <v>0.356</v>
       </c>
       <c r="H4">
-        <v>9.420999999999999</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="I4">
-        <v>1.833</v>
+        <v>1.646</v>
       </c>
       <c r="J4">
-        <v>1.853</v>
+        <v>1.81</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00108</v>
+        <v>0.00101</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -578,25 +655,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>16.754</v>
+        <v>14.29</v>
       </c>
       <c r="G5">
-        <v>0.448</v>
+        <v>0.424</v>
       </c>
       <c r="H5">
-        <v>12.085</v>
+        <v>10.034</v>
       </c>
       <c r="I5">
-        <v>2.076</v>
+        <v>1.855</v>
       </c>
       <c r="J5">
-        <v>1.981</v>
+        <v>1.837</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00102</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -616,25 +693,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>15.019</v>
+        <v>13.805</v>
       </c>
       <c r="G6">
-        <v>0.483</v>
+        <v>0.393</v>
       </c>
       <c r="H6">
-        <v>10.445</v>
+        <v>9.692</v>
       </c>
       <c r="I6">
-        <v>2.046</v>
+        <v>1.782</v>
       </c>
       <c r="J6">
-        <v>1.905</v>
+        <v>1.839</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.0009700000000000001</v>
+        <v>0.0009300000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -643,6 +720,280 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>-1.645274458028569</v>
+      </c>
+      <c r="C2">
+        <v>-23.21707356636094</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>-3.919640654934591</v>
+      </c>
+      <c r="C3">
+        <v>-2.553320925882868</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>-3.69113390607585</v>
+      </c>
+      <c r="C4">
+        <v>0.132416941088189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>10.79838647173405</v>
+      </c>
+      <c r="C5">
+        <v>-2.831068712794149e-15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>-3.187611910723564</v>
+      </c>
+      <c r="C6">
+        <v>2.420903984794039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>-15.64469938464845</v>
+      </c>
+      <c r="C7">
+        <v>-2.189579731453116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>2.273419237814216</v>
+      </c>
+      <c r="C8">
+        <v>2.382537352323087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>2.572893675100173</v>
+      </c>
+      <c r="C9">
+        <v>-0.1929576208699801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1.77635683940025e-15</v>
+      </c>
+      <c r="C10">
+        <v>1.110223024625157e-16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>-7.290197463123523</v>
+      </c>
+      <c r="C11">
+        <v>5.243063723572009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>2.605843473573495</v>
+      </c>
+      <c r="C12">
+        <v>-2.694321738188861</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>3.805859788548451</v>
+      </c>
+      <c r="C13">
+        <v>0.3998858734049386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>5.755364303716566</v>
+      </c>
+      <c r="C14">
+        <v>1.663714769400042</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>-4.876870102714975</v>
+      </c>
+      <c r="C15">
+        <v>-4.612342628188121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>1.881853646893045</v>
+      </c>
+      <c r="C16">
+        <v>1.686073766131556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>3.518868122288081</v>
+      </c>
+      <c r="C17">
+        <v>2.836849038998879</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>3.009654668471327</v>
+      </c>
+      <c r="C18">
+        <v>-2.431930382566656</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>-8.410376437652463</v>
+      </c>
+      <c r="C19">
+        <v>-2.09099242256379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>-0.02701493435443902</v>
+      </c>
+      <c r="C20">
+        <v>-0.5972006935788479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>0.6301467229078077</v>
+      </c>
+      <c r="C21">
+        <v>1.055938687732325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>0.08245388996230396</v>
+      </c>
+      <c r="C22">
+        <v>-0.1215738358437359</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>59.55094637106095</v>
+      </c>
+      <c r="C23">
+        <v>112.8474444374117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>0.05408633511067074</v>
+      </c>
+      <c r="C24">
+        <v>0.4413894059322662</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
@@ -702,25 +1053,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>13.2</v>
+        <v>111.256</v>
       </c>
       <c r="G2">
-        <v>0.008999999999999999</v>
+        <v>1.017</v>
       </c>
       <c r="H2">
-        <v>0.02</v>
+        <v>1.163</v>
       </c>
       <c r="I2">
-        <v>5.597</v>
+        <v>46.593</v>
       </c>
       <c r="J2">
-        <v>5.732</v>
+        <v>46.294</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.00117</v>
+        <v>0.00095</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -740,25 +1091,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>13.951</v>
+        <v>111.614</v>
       </c>
       <c r="G3">
-        <v>0.011</v>
+        <v>1.013</v>
       </c>
       <c r="H3">
-        <v>0.02</v>
+        <v>1.181</v>
       </c>
       <c r="I3">
-        <v>5.974</v>
+        <v>46.402</v>
       </c>
       <c r="J3">
-        <v>5.815</v>
+        <v>47.963</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00106</v>
+        <v>0.00098</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -778,25 +1129,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>13.277</v>
+        <v>114.423</v>
       </c>
       <c r="G4">
-        <v>0.008</v>
+        <v>1.022</v>
       </c>
       <c r="H4">
-        <v>0.016</v>
+        <v>1.194</v>
       </c>
       <c r="I4">
-        <v>5.692</v>
+        <v>47.634</v>
       </c>
       <c r="J4">
-        <v>5.658</v>
+        <v>47.448</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00103</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -816,25 +1167,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>13.067</v>
+        <v>112.195</v>
       </c>
       <c r="G5">
-        <v>0.008</v>
+        <v>1.016</v>
       </c>
       <c r="H5">
-        <v>0.016</v>
+        <v>1.166</v>
       </c>
       <c r="I5">
-        <v>5.523</v>
+        <v>47.836</v>
       </c>
       <c r="J5">
-        <v>5.716</v>
+        <v>47.101</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.0011</v>
+        <v>0.00098</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -854,25 +1205,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>13.976</v>
+        <v>123.969</v>
       </c>
       <c r="G6">
-        <v>0.01</v>
+        <v>1.032</v>
       </c>
       <c r="H6">
-        <v>0.02</v>
+        <v>1.192</v>
       </c>
       <c r="I6">
-        <v>6.134</v>
+        <v>50.912</v>
       </c>
       <c r="J6">
-        <v>5.898</v>
+        <v>55.727</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.00108</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -880,7 +1231,281 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>-1.645274458028569</v>
+      </c>
+      <c r="C2">
+        <v>-23.21707356636094</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>-3.919640654934591</v>
+      </c>
+      <c r="C3">
+        <v>-2.553320925882868</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>-3.69113390607585</v>
+      </c>
+      <c r="C4">
+        <v>0.132416941088189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>10.79838647173405</v>
+      </c>
+      <c r="C5">
+        <v>-2.831068712794149e-15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>-3.187611910723564</v>
+      </c>
+      <c r="C6">
+        <v>2.420903984794039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>-15.64469938464845</v>
+      </c>
+      <c r="C7">
+        <v>-2.189579731453116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>2.273419237814216</v>
+      </c>
+      <c r="C8">
+        <v>2.382537352323087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>2.572893675100173</v>
+      </c>
+      <c r="C9">
+        <v>-0.1929576208699801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1.77635683940025e-15</v>
+      </c>
+      <c r="C10">
+        <v>1.110223024625157e-16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>-7.290197463123523</v>
+      </c>
+      <c r="C11">
+        <v>5.243063723572009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>2.605843473573495</v>
+      </c>
+      <c r="C12">
+        <v>-2.694321738188861</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>3.805859788548451</v>
+      </c>
+      <c r="C13">
+        <v>0.3998858734049386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>5.755364303716566</v>
+      </c>
+      <c r="C14">
+        <v>1.663714769400042</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>-4.876870102714975</v>
+      </c>
+      <c r="C15">
+        <v>-4.612342628188121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>1.881853646893045</v>
+      </c>
+      <c r="C16">
+        <v>1.686073766131556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>3.518868122288081</v>
+      </c>
+      <c r="C17">
+        <v>2.836849038998879</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>3.009654668471327</v>
+      </c>
+      <c r="C18">
+        <v>-2.431930382566656</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>-8.410376437652463</v>
+      </c>
+      <c r="C19">
+        <v>-2.09099242256379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>-0.02701493435443902</v>
+      </c>
+      <c r="C20">
+        <v>-0.5972006935788479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>0.6301467229078077</v>
+      </c>
+      <c r="C21">
+        <v>1.055938687732325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>0.08245388996230396</v>
+      </c>
+      <c r="C22">
+        <v>-0.1215738358437359</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>59.55094637106095</v>
+      </c>
+      <c r="C23">
+        <v>112.8474444374117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>0.05408633511067074</v>
+      </c>
+      <c r="C24">
+        <v>0.4413894059322662</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -940,25 +1565,25 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>12.141</v>
+        <v>11.468</v>
       </c>
       <c r="G2">
-        <v>0.342</v>
+        <v>0.314</v>
       </c>
       <c r="H2">
-        <v>8.234999999999999</v>
+        <v>7.771</v>
       </c>
       <c r="I2">
-        <v>1.717</v>
+        <v>1.65</v>
       </c>
       <c r="J2">
-        <v>1.722</v>
+        <v>1.653</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
-        <v>0.0009300000000000001</v>
+        <v>0.00082</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -978,25 +1603,25 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>13.079</v>
+        <v>12.251</v>
       </c>
       <c r="G3">
-        <v>0.348</v>
+        <v>0.329</v>
       </c>
       <c r="H3">
-        <v>9.087999999999999</v>
+        <v>8.461</v>
       </c>
       <c r="I3">
-        <v>1.729</v>
+        <v>1.652</v>
       </c>
       <c r="J3">
-        <v>1.767</v>
+        <v>1.685</v>
       </c>
       <c r="K3">
         <v>1000</v>
       </c>
       <c r="L3">
-        <v>0.00088</v>
+        <v>0.00086</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1016,25 +1641,25 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>13.631</v>
+        <v>12.68</v>
       </c>
       <c r="G4">
-        <v>0.376</v>
+        <v>0.356</v>
       </c>
       <c r="H4">
-        <v>9.420999999999999</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="I4">
-        <v>1.833</v>
+        <v>1.646</v>
       </c>
       <c r="J4">
-        <v>1.853</v>
+        <v>1.81</v>
       </c>
       <c r="K4">
         <v>1000</v>
       </c>
       <c r="L4">
-        <v>0.00108</v>
+        <v>0.00101</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1054,25 +1679,25 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>16.754</v>
+        <v>14.29</v>
       </c>
       <c r="G5">
-        <v>0.448</v>
+        <v>0.424</v>
       </c>
       <c r="H5">
-        <v>12.085</v>
+        <v>10.034</v>
       </c>
       <c r="I5">
-        <v>2.076</v>
+        <v>1.855</v>
       </c>
       <c r="J5">
-        <v>1.981</v>
+        <v>1.837</v>
       </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>0.00102</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1092,25 +1717,25 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>15.019</v>
+        <v>13.805</v>
       </c>
       <c r="G6">
-        <v>0.483</v>
+        <v>0.393</v>
       </c>
       <c r="H6">
-        <v>10.445</v>
+        <v>9.692</v>
       </c>
       <c r="I6">
-        <v>2.046</v>
+        <v>1.782</v>
       </c>
       <c r="J6">
-        <v>1.905</v>
+        <v>1.839</v>
       </c>
       <c r="K6">
         <v>1000</v>
       </c>
       <c r="L6">
-        <v>0.0009700000000000001</v>
+        <v>0.0009300000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1130,25 +1755,25 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>13.2</v>
+        <v>111.256</v>
       </c>
       <c r="G7">
-        <v>0.008999999999999999</v>
+        <v>1.017</v>
       </c>
       <c r="H7">
-        <v>0.02</v>
+        <v>1.163</v>
       </c>
       <c r="I7">
-        <v>5.597</v>
+        <v>46.593</v>
       </c>
       <c r="J7">
-        <v>5.732</v>
+        <v>46.294</v>
       </c>
       <c r="K7">
         <v>1000</v>
       </c>
       <c r="L7">
-        <v>0.00117</v>
+        <v>0.00095</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1168,25 +1793,25 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>13.951</v>
+        <v>111.614</v>
       </c>
       <c r="G8">
-        <v>0.011</v>
+        <v>1.013</v>
       </c>
       <c r="H8">
-        <v>0.02</v>
+        <v>1.181</v>
       </c>
       <c r="I8">
-        <v>5.974</v>
+        <v>46.402</v>
       </c>
       <c r="J8">
-        <v>5.815</v>
+        <v>47.963</v>
       </c>
       <c r="K8">
         <v>1000</v>
       </c>
       <c r="L8">
-        <v>0.00106</v>
+        <v>0.00098</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1206,25 +1831,25 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>13.277</v>
+        <v>114.423</v>
       </c>
       <c r="G9">
-        <v>0.008</v>
+        <v>1.022</v>
       </c>
       <c r="H9">
-        <v>0.016</v>
+        <v>1.194</v>
       </c>
       <c r="I9">
-        <v>5.692</v>
+        <v>47.634</v>
       </c>
       <c r="J9">
-        <v>5.658</v>
+        <v>47.448</v>
       </c>
       <c r="K9">
         <v>1000</v>
       </c>
       <c r="L9">
-        <v>0.00103</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1244,25 +1869,25 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>13.067</v>
+        <v>112.195</v>
       </c>
       <c r="G10">
-        <v>0.008</v>
+        <v>1.016</v>
       </c>
       <c r="H10">
-        <v>0.016</v>
+        <v>1.166</v>
       </c>
       <c r="I10">
-        <v>5.523</v>
+        <v>47.836</v>
       </c>
       <c r="J10">
-        <v>5.716</v>
+        <v>47.101</v>
       </c>
       <c r="K10">
         <v>1000</v>
       </c>
       <c r="L10">
-        <v>0.0011</v>
+        <v>0.00098</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1282,25 +1907,25 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>13.976</v>
+        <v>123.969</v>
       </c>
       <c r="G11">
-        <v>0.01</v>
+        <v>1.032</v>
       </c>
       <c r="H11">
-        <v>0.02</v>
+        <v>1.192</v>
       </c>
       <c r="I11">
-        <v>6.134</v>
+        <v>50.912</v>
       </c>
       <c r="J11">
-        <v>5.898</v>
+        <v>55.727</v>
       </c>
       <c r="K11">
         <v>1000</v>
       </c>
       <c r="L11">
-        <v>0.00108</v>
+        <v>0.0009700000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>